<commit_message>
Agregado de la sección Preguntas
</commit_message>
<xml_diff>
--- a/RCLV.xlsx
+++ b/RCLV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="4575" tabRatio="818" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="4575" tabRatio="818" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Subcats CFC - Cuestionario" sheetId="3" r:id="rId1"/>
@@ -971,12 +971,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -1021,6 +1015,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1316,7 +1316,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -1324,66 +1324,66 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="82" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="84" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="88" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="90" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="90" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="93" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="97" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1436,7 +1436,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
+      <c r="A4" s="97"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1456,7 +1456,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="97"/>
       <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="98" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1475,7 +1475,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1542,16 +1542,16 @@
       <c r="F1" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="94" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="94" t="s">
         <v>116</v>
       </c>
       <c r="K1" s="66" t="s">
@@ -2018,13 +2018,13 @@
       <c r="D1" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="95" t="s">
         <v>46</v>
       </c>
       <c r="H1" s="74" t="s">
@@ -2337,7 +2337,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2366,16 +2366,16 @@
       <c r="D1" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="F1" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="G1" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="H1" s="96" t="s">
         <v>52</v>
       </c>
       <c r="I1" s="65" t="s">
@@ -2685,8 +2685,8 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,28 +2896,24 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="21"/>
       <c r="G17" s="28" t="s">
         <v>61</v>
       </c>
       <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
       <c r="H18" s="44"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
       <c r="F19" s="15" t="s">
         <v>38</v>
       </c>

</xml_diff>